<commit_message>
add `$.num.` prefix for avoiding the string value in json of decimal value from database.
upgrade mysql2 and typeorm
</commit_message>
<xml_diff>
--- a/o23-n6/test/template.xlsx
+++ b/o23-n6/test/template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF9D700-889D-3448-94D5-B801110F5661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF52A26-B878-E84F-8C1B-0BB109ABF89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,10 +14,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$5:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -121,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>SUMMARY OF TOTAL COLLECTIONS - SGD</t>
   </si>
@@ -170,10 +180,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$subTotal.cashInTxn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$subTotal.cashInAmt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,10 +204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$cashInTxnTotal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$cashInAmtTotal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -218,6 +220,9 @@
   </si>
   <si>
     <t>$.$del</t>
+  </si>
+  <si>
+    <t>$.num.subTotal.cashInTxn</t>
   </si>
 </sst>
 </file>
@@ -309,16 +314,16 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +612,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -618,23 +623,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="78" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -643,21 +648,21 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="107" customHeight="1">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -671,27 +676,28 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4">
+        <f ca="1">SUM(OFFSET(D$5,0,0,ROW()-5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -707,24 +713,24 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>